<commit_message>
Stubs & Use Casses
</commit_message>
<xml_diff>
--- a/BackEndLogic-Stubs/Use Casses.xlsx
+++ b/BackEndLogic-Stubs/Use Casses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t xml:space="preserve">Requests </t>
   </si>
@@ -306,6 +306,33 @@
   </si>
   <si>
     <t>All deliverd jobs , Total No. of deliverd jobs , Total No. of Pages</t>
+  </si>
+  <si>
+    <t>connectcollect.com/forgot_password/</t>
+  </si>
+  <si>
+    <t>User Email</t>
+  </si>
+  <si>
+    <t>it check email and then send code to user email address</t>
+  </si>
+  <si>
+    <t>connectcollect.com/password_reset/</t>
+  </si>
+  <si>
+    <t>User Email, varification Code</t>
+  </si>
+  <si>
+    <t>connectcollect.com/verify_password_reset_code/</t>
+  </si>
+  <si>
+    <t>User Email, varification Code, New Password</t>
+  </si>
+  <si>
+    <t>connectcollect.com/editt_credit_card_address_info/</t>
+  </si>
+  <si>
+    <t>Houser number, Street, Town/City, County, Postcode, Country, User_ID, Address_ID</t>
   </si>
 </sst>
 </file>
@@ -626,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,6 +1226,48 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>102</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update stubs & DB
</commit_message>
<xml_diff>
--- a/BackEndLogic-Stubs/Use Casses.xlsx
+++ b/BackEndLogic-Stubs/Use Casses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t xml:space="preserve">Requests </t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>/password_reset/</t>
+  </si>
+  <si>
+    <t>/jobs_for_map_view/</t>
+  </si>
+  <si>
+    <t>courier_counties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jobs short details </t>
   </si>
 </sst>
 </file>
@@ -653,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,10 +1033,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>104</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1035,10 +1047,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,10 +1058,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,10 +1069,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1068,10 +1080,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1079,10 +1091,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,10 +1102,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1101,13 +1113,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1115,13 +1124,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1129,13 +1138,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,13 +1152,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1157,13 +1166,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1171,13 +1180,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,13 +1194,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,13 +1208,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,13 +1222,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1227,45 +1236,56 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>54</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>